<commit_message>
hit probability looks better now
</commit_message>
<xml_diff>
--- a/ribs.xlsx
+++ b/ribs.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dejan\Documents\Repositories\Local\rust101\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dejan\Documents\Repositories\GitHub\ribs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB819D8-2189-48B7-9AF8-F8E55711DBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E381B2D2-CA70-42ED-9A42-85AF19659D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30075" yWindow="855" windowWidth="34545" windowHeight="15435" xr2:uid="{D8DE7F68-55FF-48AD-AF63-E0E4AE38E202}"/>
+    <workbookView xWindow="5340" yWindow="3750" windowWidth="34545" windowHeight="15435" activeTab="1" xr2:uid="{D8DE7F68-55FF-48AD-AF63-E0E4AE38E202}"/>
   </bookViews>
   <sheets>
     <sheet name="Hit chance" sheetId="1" r:id="rId1"/>
+    <sheet name="Hit chance 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,19 +37,136 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="38">
   <si>
     <t>Player/Min_req</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>0.45</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>0.35</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.15000000000000002</t>
+  </si>
+  <si>
+    <t>0.09999999999999998</t>
+  </si>
+  <si>
+    <t>0.04999999999999999</t>
+  </si>
+  <si>
+    <t> 0</t>
+  </si>
+  <si>
+    <t> 0.04999999999999999</t>
+  </si>
+  <si>
+    <t> 0.09999999999999998</t>
+  </si>
+  <si>
+    <t> 0.15000000000000002</t>
+  </si>
+  <si>
+    <t> 0.2</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
+    <t> 0.25</t>
+  </si>
+  <si>
+    <t>0.65</t>
+  </si>
+  <si>
+    <t> 0.3</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t> 0.35</t>
+  </si>
+  <si>
+    <t>0.8500000000000001</t>
+  </si>
+  <si>
+    <t> 0.4</t>
+  </si>
+  <si>
+    <t>0.9500000000000001</t>
+  </si>
+  <si>
+    <t> 0.45</t>
+  </si>
+  <si>
+    <t> 1</t>
+  </si>
+  <si>
+    <t> 2</t>
+  </si>
+  <si>
+    <t> 3</t>
+  </si>
+  <si>
+    <t> 4</t>
+  </si>
+  <si>
+    <t> 5</t>
+  </si>
+  <si>
+    <t> 6</t>
+  </si>
+  <si>
+    <t> 7</t>
+  </si>
+  <si>
+    <t> 8</t>
+  </si>
+  <si>
+    <t> 9</t>
+  </si>
+  <si>
+    <t>Me</t>
+  </si>
+  <si>
+    <t>Minimal requirements</t>
+  </si>
+  <si>
+    <t>Hit probability</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,9 +198,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,7 +522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4004151-A81B-43BC-98AE-EAFABF6686B0}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -619,4 +742,1367 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E15384-2EF3-4102-A067-75DC18EE7319}">
+  <dimension ref="A1:C122"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60:C60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>2</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>3</v>
+      </c>
+      <c r="B42">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>4</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>4</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>4</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>4</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <v>6</v>
+      </c>
+      <c r="C52" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>4</v>
+      </c>
+      <c r="B53">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>4</v>
+      </c>
+      <c r="B54">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>4</v>
+      </c>
+      <c r="B55">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>4</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>5</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>5</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <v>5</v>
+      </c>
+      <c r="B62">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <v>5</v>
+      </c>
+      <c r="B63">
+        <v>6</v>
+      </c>
+      <c r="C63" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
+        <v>5</v>
+      </c>
+      <c r="B64">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <v>5</v>
+      </c>
+      <c r="B65">
+        <v>8</v>
+      </c>
+      <c r="C65" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>5</v>
+      </c>
+      <c r="B66">
+        <v>9</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <v>5</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>6</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>6</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>6</v>
+      </c>
+      <c r="B70">
+        <v>2</v>
+      </c>
+      <c r="C70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>6</v>
+      </c>
+      <c r="B71">
+        <v>3</v>
+      </c>
+      <c r="C71" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>6</v>
+      </c>
+      <c r="B72">
+        <v>4</v>
+      </c>
+      <c r="C72" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>6</v>
+      </c>
+      <c r="B73">
+        <v>5</v>
+      </c>
+      <c r="C73" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>6</v>
+      </c>
+      <c r="B74">
+        <v>6</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>6</v>
+      </c>
+      <c r="B75">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>6</v>
+      </c>
+      <c r="B76">
+        <v>8</v>
+      </c>
+      <c r="C76" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
+        <v>6</v>
+      </c>
+      <c r="B77">
+        <v>9</v>
+      </c>
+      <c r="C77" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>6</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <v>7</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <v>7</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <v>7</v>
+      </c>
+      <c r="B81">
+        <v>2</v>
+      </c>
+      <c r="C81" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
+        <v>7</v>
+      </c>
+      <c r="B82">
+        <v>3</v>
+      </c>
+      <c r="C82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
+        <v>7</v>
+      </c>
+      <c r="B83">
+        <v>4</v>
+      </c>
+      <c r="C83" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="4">
+        <v>7</v>
+      </c>
+      <c r="B84">
+        <v>5</v>
+      </c>
+      <c r="C84" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>7</v>
+      </c>
+      <c r="B85">
+        <v>6</v>
+      </c>
+      <c r="C85" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
+        <v>7</v>
+      </c>
+      <c r="B86">
+        <v>7</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="4">
+        <v>7</v>
+      </c>
+      <c r="B87">
+        <v>8</v>
+      </c>
+      <c r="C87" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="4">
+        <v>7</v>
+      </c>
+      <c r="B88">
+        <v>9</v>
+      </c>
+      <c r="C88" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
+        <v>7</v>
+      </c>
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="4">
+        <v>8</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="4">
+        <v>8</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
+        <v>8</v>
+      </c>
+      <c r="B92">
+        <v>2</v>
+      </c>
+      <c r="C92">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="4">
+        <v>8</v>
+      </c>
+      <c r="B93">
+        <v>3</v>
+      </c>
+      <c r="C93">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
+        <v>8</v>
+      </c>
+      <c r="B94">
+        <v>4</v>
+      </c>
+      <c r="C94">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="4">
+        <v>8</v>
+      </c>
+      <c r="B95">
+        <v>5</v>
+      </c>
+      <c r="C95">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="4">
+        <v>8</v>
+      </c>
+      <c r="B96">
+        <v>6</v>
+      </c>
+      <c r="C96">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="4">
+        <v>8</v>
+      </c>
+      <c r="B97">
+        <v>7</v>
+      </c>
+      <c r="C97">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>8</v>
+      </c>
+      <c r="B98">
+        <v>8</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="4">
+        <v>8</v>
+      </c>
+      <c r="B99">
+        <v>9</v>
+      </c>
+      <c r="C99" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="4">
+        <v>8</v>
+      </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
+      <c r="C100" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="4">
+        <v>9</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+      <c r="C101" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="4">
+        <v>9</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="4">
+        <v>9</v>
+      </c>
+      <c r="B103">
+        <v>2</v>
+      </c>
+      <c r="C103" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="4">
+        <v>9</v>
+      </c>
+      <c r="B104">
+        <v>3</v>
+      </c>
+      <c r="C104" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="4">
+        <v>9</v>
+      </c>
+      <c r="B105">
+        <v>4</v>
+      </c>
+      <c r="C105" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="4">
+        <v>9</v>
+      </c>
+      <c r="B106">
+        <v>5</v>
+      </c>
+      <c r="C106" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="4">
+        <v>9</v>
+      </c>
+      <c r="B107">
+        <v>6</v>
+      </c>
+      <c r="C107" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="4">
+        <v>9</v>
+      </c>
+      <c r="B108">
+        <v>7</v>
+      </c>
+      <c r="C108" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="4">
+        <v>9</v>
+      </c>
+      <c r="B109">
+        <v>8</v>
+      </c>
+      <c r="C109" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="4">
+        <v>9</v>
+      </c>
+      <c r="B110">
+        <v>9</v>
+      </c>
+      <c r="C110" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="4">
+        <v>9</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="C111" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="4">
+        <v>1</v>
+      </c>
+      <c r="B112" t="s">
+        <v>11</v>
+      </c>
+      <c r="C112" s="2">
+        <v>45047</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="4">
+        <v>1</v>
+      </c>
+      <c r="B113" t="s">
+        <v>26</v>
+      </c>
+      <c r="C113" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="4">
+        <v>1</v>
+      </c>
+      <c r="B114" t="s">
+        <v>27</v>
+      </c>
+      <c r="C114" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="4">
+        <v>1</v>
+      </c>
+      <c r="B115" t="s">
+        <v>28</v>
+      </c>
+      <c r="C115" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="4">
+        <v>1</v>
+      </c>
+      <c r="B116" t="s">
+        <v>29</v>
+      </c>
+      <c r="C116" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="4">
+        <v>1</v>
+      </c>
+      <c r="B117" t="s">
+        <v>30</v>
+      </c>
+      <c r="C117" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="4">
+        <v>1</v>
+      </c>
+      <c r="B118" t="s">
+        <v>31</v>
+      </c>
+      <c r="C118" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="4">
+        <v>1</v>
+      </c>
+      <c r="B119" t="s">
+        <v>32</v>
+      </c>
+      <c r="C119" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="4">
+        <v>1</v>
+      </c>
+      <c r="B120" t="s">
+        <v>33</v>
+      </c>
+      <c r="C120" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="4">
+        <v>1</v>
+      </c>
+      <c r="B121" t="s">
+        <v>34</v>
+      </c>
+      <c r="C121" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="4">
+        <v>1</v>
+      </c>
+      <c r="B122" t="s">
+        <v>26</v>
+      </c>
+      <c r="C122" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>